<commit_message>
nnuevas funciones y main creado
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>dni</t>
   </si>
@@ -31,6 +31,9 @@
     <t>admin</t>
   </si>
   <si>
+    <t>66admin66</t>
+  </si>
+  <si>
     <t>account</t>
   </si>
   <si>
@@ -38,6 +41,9 @@
   </si>
   <si>
     <t>owner</t>
+  </si>
+  <si>
+    <t>0cc447ac8b9791feaddb339c7a63256a</t>
   </si>
 </sst>
 </file>
@@ -355,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +383,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -384,23 +401,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>